<commit_message>
E2 SKU pricing Added
</commit_message>
<xml_diff>
--- a/gcp-sku-pricing.xlsx
+++ b/gcp-sku-pricing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jainmudit/Documents/pricing package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jainmudit/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B9B0B-6A19-754E-B9A0-903D4D42FBAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC956ACF-1251-CE45-8E9F-533F90FD5F96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" activeTab="3" xr2:uid="{57DC3CAE-9CC7-C14F-855D-4F25333067E3}"/>
+    <workbookView xWindow="2720" yWindow="3200" windowWidth="27240" windowHeight="15940" activeTab="5" xr2:uid="{57DC3CAE-9CC7-C14F-855D-4F25333067E3}"/>
   </bookViews>
   <sheets>
     <sheet name="ap-south1-pricing" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="SOT" sheetId="6" r:id="rId3"/>
     <sheet name="SOT-N2" sheetId="7" r:id="rId4"/>
     <sheet name="global license pricing" sheetId="5" r:id="rId5"/>
+    <sheet name="SOT-E2" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ap-south1-pricing'!$A$1:$M$35</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="171">
   <si>
     <t>skus__skus__description</t>
   </si>
@@ -539,6 +540,15 @@
   </si>
   <si>
     <t>N2_custom_core_3yr</t>
+  </si>
+  <si>
+    <t>E2_custom_core_on-deman</t>
+  </si>
+  <si>
+    <t>E2_custom_core_1yr</t>
+  </si>
+  <si>
+    <t>E2_custom_core_3yr</t>
   </si>
 </sst>
 </file>
@@ -3077,7 +3087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7166E874-AC44-2346-A038-1F316533BA43}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -3787,4 +3797,582 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9B257F-61E3-124D-8CF9-EE596CF03996}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2">
+        <v>3.38514E-3</v>
+      </c>
+      <c r="D2">
+        <v>2.1326380000000001E-3</v>
+      </c>
+      <c r="E2">
+        <v>1.5233130000000001E-3</v>
+      </c>
+      <c r="F2">
+        <v>2.5255380000000001E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.5910889000000001E-2</v>
+      </c>
+      <c r="H2">
+        <v>1.1364921E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3">
+        <v>2.9235300000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>1.841823E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.3155879999999999E-3</v>
+      </c>
+      <c r="F3">
+        <v>2.1811589999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.3741300999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>9.8152150000000004E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>3.21609E-3</v>
+      </c>
+      <c r="D4">
+        <v>2.026136E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.44724E-3</v>
+      </c>
+      <c r="F4">
+        <v>2.399337E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.5115823E-2</v>
+      </c>
+      <c r="H4">
+        <v>1.0797016E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5">
+        <v>3.2181599999999999E-3</v>
+      </c>
+      <c r="D5">
+        <v>2.0274400000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>1.448172E-3</v>
+      </c>
+      <c r="F5">
+        <v>2.4016139999999998E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.5130167999999999E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.0807262999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6">
+        <v>3.7660200000000001E-3</v>
+      </c>
+      <c r="D6">
+        <v>2.3725920000000002E-3</v>
+      </c>
+      <c r="E6">
+        <v>1.694709E-3</v>
+      </c>
+      <c r="F6">
+        <v>2.8103699999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.7705331000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>1.2646665E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7">
+        <v>4.0903199999999997E-3</v>
+      </c>
+      <c r="D7">
+        <v>2.5769009999999999E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.840644E-3</v>
+      </c>
+      <c r="F7">
+        <v>3.051939E-2</v>
+      </c>
+      <c r="G7">
+        <v>1.9227214999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.3733725E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <v>3.9304739999999998E-3</v>
+      </c>
+      <c r="D8">
+        <v>2.4761980000000002E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.7687130000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>2.9331146999999998E-2</v>
+      </c>
+      <c r="G8">
+        <v>1.8478628E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.3199017E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9">
+        <v>3.7391099999999999E-3</v>
+      </c>
+      <c r="D9">
+        <v>2.3556390000000001E-3</v>
+      </c>
+      <c r="E9">
+        <v>1.6825989999999999E-3</v>
+      </c>
+      <c r="F9">
+        <v>2.802642E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.7656643999999999E-2</v>
+      </c>
+      <c r="H9">
+        <v>1.2611888999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10">
+        <v>3.2919899999999998E-3</v>
+      </c>
+      <c r="D10">
+        <v>2.0739529999999999E-3</v>
+      </c>
+      <c r="E10">
+        <v>1.4813949999999999E-3</v>
+      </c>
+      <c r="F10">
+        <v>2.4567450000000001E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.5477493E-2</v>
+      </c>
+      <c r="H10">
+        <v>1.1055351999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>3.7660200000000001E-3</v>
+      </c>
+      <c r="D11">
+        <v>2.3725920000000002E-3</v>
+      </c>
+      <c r="E11">
+        <v>1.694709E-3</v>
+      </c>
+      <c r="F11">
+        <v>2.8103699999999999E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.7705331000000001E-2</v>
+      </c>
+      <c r="H11">
+        <v>1.2646665E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12">
+        <v>3.51141E-3</v>
+      </c>
+      <c r="D12">
+        <v>2.2121879999999999E-3</v>
+      </c>
+      <c r="E12">
+        <v>1.580134E-3</v>
+      </c>
+      <c r="F12">
+        <v>2.6199299999999998E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.6505559E-2</v>
+      </c>
+      <c r="H12">
+        <v>1.1789684999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13">
+        <v>3.2181599999999999E-3</v>
+      </c>
+      <c r="D13">
+        <v>2.0274400000000001E-3</v>
+      </c>
+      <c r="E13">
+        <v>1.448172E-3</v>
+      </c>
+      <c r="F13">
+        <v>2.4013380000000001E-2</v>
+      </c>
+      <c r="G13">
+        <v>1.5128429000000001E-2</v>
+      </c>
+      <c r="H13">
+        <v>1.0806021000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14">
+        <v>3.5107200000000002E-3</v>
+      </c>
+      <c r="D14">
+        <v>2.2117529999999999E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.5798240000000001E-3</v>
+      </c>
+      <c r="F14">
+        <v>2.6199299999999998E-2</v>
+      </c>
+      <c r="G14">
+        <v>1.6505559E-2</v>
+      </c>
+      <c r="H14">
+        <v>1.1789684999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>3.2181599999999999E-3</v>
+      </c>
+      <c r="D15">
+        <v>2.0274400000000001E-3</v>
+      </c>
+      <c r="E15">
+        <v>1.448172E-3</v>
+      </c>
+      <c r="F15">
+        <v>2.4013380000000001E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.5128429000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>1.0806021000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16">
+        <v>3.7391099999999999E-3</v>
+      </c>
+      <c r="D16">
+        <v>2.3556390000000001E-3</v>
+      </c>
+      <c r="E16">
+        <v>1.6825989999999999E-3</v>
+      </c>
+      <c r="F16">
+        <v>2.802642E-2</v>
+      </c>
+      <c r="G16">
+        <v>1.7656643999999999E-2</v>
+      </c>
+      <c r="H16">
+        <v>1.2611888999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17">
+        <v>3.51141E-3</v>
+      </c>
+      <c r="D17">
+        <v>2.2121879999999999E-3</v>
+      </c>
+      <c r="E17">
+        <v>1.580134E-3</v>
+      </c>
+      <c r="F17">
+        <v>2.6199299999999998E-2</v>
+      </c>
+      <c r="G17">
+        <v>1.6505559E-2</v>
+      </c>
+      <c r="H17">
+        <v>1.1789684999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18">
+        <v>4.6402500000000003E-3</v>
+      </c>
+      <c r="D18">
+        <v>2.9233570000000001E-3</v>
+      </c>
+      <c r="E18">
+        <v>2.088112E-3</v>
+      </c>
+      <c r="F18">
+        <v>3.4624200000000001E-2</v>
+      </c>
+      <c r="G18">
+        <v>2.1813246000000001E-2</v>
+      </c>
+      <c r="H18">
+        <v>1.558089E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19">
+        <v>3.7391099999999999E-3</v>
+      </c>
+      <c r="D19">
+        <v>2.3556390000000001E-3</v>
+      </c>
+      <c r="E19">
+        <v>1.6825989999999999E-3</v>
+      </c>
+      <c r="F19">
+        <v>2.802642E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.7656643999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.2611888999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20">
+        <v>3.6059400000000002E-3</v>
+      </c>
+      <c r="D20">
+        <v>2.2717420000000002E-3</v>
+      </c>
+      <c r="E20">
+        <v>1.622673E-3</v>
+      </c>
+      <c r="F20">
+        <v>2.6909309999999999E-2</v>
+      </c>
+      <c r="G20">
+        <v>1.6952865000000001E-2</v>
+      </c>
+      <c r="H20">
+        <v>1.2109188999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21">
+        <v>4.1475899999999996E-3</v>
+      </c>
+      <c r="D21">
+        <v>2.6129809999999999E-3</v>
+      </c>
+      <c r="E21">
+        <v>1.866415E-3</v>
+      </c>
+      <c r="F21">
+        <v>3.0950640000000001E-2</v>
+      </c>
+      <c r="G21">
+        <v>1.9498903000000001E-2</v>
+      </c>
+      <c r="H21">
+        <v>1.3927788E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22">
+        <v>3.2919899999999998E-3</v>
+      </c>
+      <c r="D22">
+        <v>2.0739529999999999E-3</v>
+      </c>
+      <c r="E22">
+        <v>1.4813949999999999E-3</v>
+      </c>
+      <c r="F22">
+        <v>2.4567450000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>1.5477493E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.1055351999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23">
+        <v>3.7660200000000001E-3</v>
+      </c>
+      <c r="D23">
+        <v>2.3725920000000002E-3</v>
+      </c>
+      <c r="E23">
+        <v>1.694709E-3</v>
+      </c>
+      <c r="F23">
+        <v>2.8103699999999999E-2</v>
+      </c>
+      <c r="G23">
+        <v>1.7705331000000001E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.2646665E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24">
+        <v>4.0903199999999997E-3</v>
+      </c>
+      <c r="D24">
+        <v>2.5769009999999999E-3</v>
+      </c>
+      <c r="E24">
+        <v>1.840644E-3</v>
+      </c>
+      <c r="F24">
+        <v>3.051939E-2</v>
+      </c>
+      <c r="G24">
+        <v>1.9227214999999999E-2</v>
+      </c>
+      <c r="H24">
+        <v>1.3733725E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>